<commit_message>
final updates on the application
</commit_message>
<xml_diff>
--- a/FeedbackForm.xlsx
+++ b/FeedbackForm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyan\Documents\UiPath\Newfolder\AIPriceComparisonApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53431A77-809D-41EB-808C-CCE5BC2E03AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE3B01D-E972-4F86-B352-123575A66FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="20910" windowHeight="11835" xr2:uid="{91493344-386A-4763-BE0D-8443CDECC2E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{91493344-386A-4763-BE0D-8443CDECC2E4}"/>
   </bookViews>
   <sheets>
     <sheet name="PieChart_CustomerReview" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -117,16 +117,70 @@
     <t>Happy with this application</t>
   </si>
   <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>T@</t>
+  </si>
+  <si>
+    <t>hAPPY</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Need improvement</t>
+  </si>
+  <si>
+    <t>Disapointed</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Jesmond</t>
+  </si>
+  <si>
+    <t>jesmond@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Too slow </t>
+  </si>
+  <si>
+    <t>Melvin</t>
+  </si>
+  <si>
+    <t>melvin@gmail.com</t>
+  </si>
+  <si>
+    <t>Very happy</t>
+  </si>
+  <si>
+    <t>Very Positive</t>
+  </si>
+  <si>
+    <t>sheila@gmail.com</t>
+  </si>
+  <si>
+    <t>Disappointed</t>
+  </si>
+  <si>
+    <t>Verrryyyyy happy</t>
+  </si>
+  <si>
     <t>Row Labels</t>
   </si>
   <si>
     <t>Count of Sentiment</t>
   </si>
   <si>
+    <t>(blank)</t>
+  </si>
+  <si>
     <t>Grand Total</t>
-  </si>
-  <si>
-    <t>(blank)</t>
   </si>
 </sst>
 </file>
@@ -210,6 +264,296 @@
       <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Total</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>Positive</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Very Negative</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Neutral</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Negative</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Very Positive</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>(blank)</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>0</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C668-4854-A726-1B20C042B10B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Total</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>Positive</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Very Negative</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Neutral</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Negative</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Very Positive</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>(blank)</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>0</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4E3A-414E-8DC6-858158B0CEA2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:pivotSource>
     <c:name>[FeedbackForm.xlsx]PieChart_CustomerReview!Pie Data</c:name>
     <c:fmtId val="0"/>
@@ -254,16 +598,25 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>PieChart_CustomerReview!$A$2:$A$5</c:f>
+              <c:f>PieChart_CustomerReview!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>Negative</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neutral</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Positive</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>Very Negative</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>Very Positive</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>(blank)</c:v>
                 </c:pt>
               </c:strCache>
@@ -271,14 +624,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PieChart_CustomerReview!$B$2:$B$5</c:f>
+              <c:f>PieChart_CustomerReview!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -286,7 +648,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5647-4543-A895-F93ED00A6B4C}"/>
+              <c16:uniqueId val="{00000000-43F2-4834-99E2-9EADF6547020}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -345,23 +707,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>111125</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D64EDFF-8EB7-8FD5-4F22-CFA2197A9E5E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D30E0A04-8BD0-16C0-82C0-E9DE6A351D91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -379,13 +741,85 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28D39603-42A1-CF07-7F5A-F4FE69B518E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BFC24F3-1B95-655B-FA74-E6AE219E4A01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Chan Cyan" refreshedDate="44966.007933912035" createdVersion="1" refreshedVersion="8" recordCount="8" xr:uid="{FD0F6160-B9D1-4B86-A813-1D2D4CCE5451}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Chan Cyan" refreshedDate="44966.469323263889" createdVersion="1" refreshedVersion="8" recordCount="15" xr:uid="{11B96E43-A9FC-422B-99C1-263BDA25E99C}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:D9" sheet="UiPathForm"/>
+    <worksheetSource ref="A1:D16" sheet="UiPathForm"/>
   </cacheSource>
   <cacheFields count="4">
     <cacheField name="Name" numFmtId="0">
@@ -398,10 +832,13 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="Sentiment" numFmtId="0">
-      <sharedItems containsBlank="1" count="3">
+      <sharedItems containsBlank="1" count="6">
         <s v="Positive"/>
         <s v="Very Negative"/>
         <m/>
+        <s v="Neutral"/>
+        <s v="Negative"/>
+        <s v="Very Positive"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -414,7 +851,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="8">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="15">
   <r>
     <s v="Sheila"/>
     <s v="Test"/>
@@ -463,12 +900,54 @@
     <s v="Happy with this application"/>
     <x v="0"/>
   </r>
+  <r>
+    <s v="t"/>
+    <s v="T@"/>
+    <s v="hAPPY"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="t"/>
+    <s v="T"/>
+    <s v="Need improvement"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Cyan"/>
+    <s v="cyan@gmail.com"/>
+    <s v="Disapointed"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Jesmond"/>
+    <s v="jesmond@gmail.com"/>
+    <s v="Too slow "/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Melvin"/>
+    <s v="melvin@gmail.com"/>
+    <s v="Very happy"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="Sheila"/>
+    <s v="sheila@gmail.com"/>
+    <s v="Disappointed"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Cyan"/>
+    <s v="cyan@gmail.com"/>
+    <s v="Verrryyyyy happy"/>
+    <x v="3"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{15C0D73E-84D8-4781-9EF0-FC11C5F34FEF}" name="Pie Data" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" pageOverThenDown="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1" chartFormat="1">
-  <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AEF3AE42-0112-4168-B43C-1B7166DFC33E}" name="Pie Data" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" pageOverThenDown="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1" chartFormat="1">
+  <location ref="A1:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0" includeNewItemsInFilter="1">
       <extLst>
@@ -492,9 +971,12 @@
       </extLst>
     </pivotField>
     <pivotField axis="axisRow" dataField="1" showAll="0" includeNewItemsInFilter="1">
-      <items count="4">
+      <items count="7">
+        <item x="4"/>
+        <item x="3"/>
         <item x="0"/>
         <item x="1"/>
+        <item x="5"/>
         <item x="2"/>
         <item t="default"/>
       </items>
@@ -508,7 +990,7 @@
   <rowFields count="1">
     <field x="3"/>
   </rowFields>
-  <rowItems count="4">
+  <rowItems count="7">
     <i>
       <x/>
     </i>
@@ -517,6 +999,15 @@
     </i>
     <i>
       <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
     </i>
     <i t="grand">
       <x/>
@@ -848,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80E178-60CB-41AE-801C-CD403328AD92}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,15 +1353,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -878,24 +1369,48 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4">
-        <v>3</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="4">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -906,10 +1421,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,6 +1545,104 @@
         <v>7</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>

<commit_message>
finalised flowchart & minor updates
</commit_message>
<xml_diff>
--- a/FeedbackForm.xlsx
+++ b/FeedbackForm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyan\Documents\UiPath\Newfolder\AIPriceComparisonApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B0E9D0-09D9-48E7-A812-75624DE13C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2839C7-BD6C-42F3-96A0-31690A9F1FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="2025" windowWidth="20910" windowHeight="11835" xr2:uid="{91493344-386A-4763-BE0D-8443CDECC2E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{91493344-386A-4763-BE0D-8443CDECC2E4}"/>
   </bookViews>
   <sheets>
     <sheet name="PieChart_CustomerReview" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -180,20 +180,13 @@
     <t>Happy</t>
   </si>
   <si>
-    <t xml:space="preserve">Happy
-</t>
-  </si>
-  <si>
-    <t>{Error : : predict processes one line at a time (remove '\\n')}</t>
+    <t>Need Improvement but still happy to use this application</t>
   </si>
   <si>
     <t>Row Labels</t>
   </si>
   <si>
     <t>Count of Sentiment</t>
-  </si>
-  <si>
-    <t>(blank)</t>
   </si>
   <si>
     <t>Grand Total</t>
@@ -267,762 +260,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:delete val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="1"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:delete val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-    </c:pivotFmts>
-    <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Total</c:v>
-          </c:tx>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="6"/>
-              <c:pt idx="0">
-                <c:v>Positive</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Very Negative</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Neutral</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Negative</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Very Positive</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>(blank)</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="6"/>
-              <c:pt idx="0">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>1</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>4</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>1</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>0</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5BFB-4BE8-BEB5-636B007C64B7}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:extLst/>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:delete val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="1"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:delete val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-    </c:pivotFmts>
-    <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Total</c:v>
-          </c:tx>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="6"/>
-              <c:pt idx="0">
-                <c:v>Positive</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Very Negative</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Neutral</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Negative</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Very Positive</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>(blank)</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="6"/>
-              <c:pt idx="0">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>1</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>5</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>1</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>0</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7999-4B1F-87A0-F80B6A928C02}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:extLst/>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:delete val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="1"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:delete val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-    </c:pivotFmts>
-    <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Total</c:v>
-          </c:tx>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="6"/>
-              <c:pt idx="0">
-                <c:v>Positive</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Very Negative</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Neutral</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Negative</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Very Positive</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>(blank)</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="6"/>
-              <c:pt idx="0">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>1</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>7</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>1</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>0</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-37F7-42B3-92EB-29F0C49D467F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:extLst/>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:pivotSource>
-    <c:name>[FeedbackForm.xlsx]PieChart_CustomerReview!Pie Data</c:name>
-    <c:fmtId val="0"/>
-  </c:pivotSource>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:delete val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-    </c:pivotFmts>
-    <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>PieChart_CustomerReview!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>PieChart_CustomerReview!$A$2:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>{Error : : predict processes one line at a time (remove '\\n')}</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Negative</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Neutral</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Positive</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Very Negative</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Very Positive</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>(blank)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>PieChart_CustomerReview!$B$2:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BA4E-4D9E-B6C1-D97CDF4EED7E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:extLst>
-    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
-      <c14:pivotOptions>
-        <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
-        <c14:dropZoneSeries val="1"/>
-        <c14:dropZonesVisible val="1"/>
-      </c14:pivotOptions>
-    </c:ext>
-    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
-      <c16:pivotOptions16>
-        <c16:showExpandCollapseFieldButtons val="1"/>
-      </c16:pivotOptions16>
-    </c:ext>
-  </c:extLst>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>327025</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BFC24F3-1B95-655B-FA74-E6AE219E4A01}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6397C57-640E-CA41-DA00-A70C85C24D3E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2D7BD6F-DDA7-0607-1FAD-214ACB338A14}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>374650</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88086FAF-0AFC-8014-A336-5690934054CA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Chan Cyan" refreshedDate="44969.636630208333" createdVersion="1" refreshedVersion="8" recordCount="19" xr:uid="{1F4EB0CE-95E0-4B2C-AF3E-37F048F9FB18}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Chan Cyan" refreshedDate="44969.901609490742" createdVersion="1" refreshedVersion="8" recordCount="20" xr:uid="{3CEE1FB9-A687-4BBE-9173-84BA216B5666}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:D20" sheet="UiPathForm"/>
+    <worksheetSource ref="A1:D21" sheet="UiPathForm"/>
   </cacheSource>
   <cacheFields count="4">
     <cacheField name="Name" numFmtId="0">
@@ -1035,14 +276,12 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="Sentiment" numFmtId="0">
-      <sharedItems containsBlank="1" count="7">
+      <sharedItems count="5">
         <s v="Positive"/>
         <s v="Very Negative"/>
-        <m/>
         <s v="Neutral"/>
         <s v="Negative"/>
         <s v="Very Positive"/>
-        <s v="{Error : : predict processes one line at a time (remove '\\n')}"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -1055,7 +294,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="19">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="20">
   <r>
     <s v="Sheila"/>
     <s v="Test"/>
@@ -1072,31 +311,31 @@
     <s v="George"/>
     <s v="sheilalyt@gmail.com"/>
     <s v="I'm staticfied with the service "/>
-    <x v="2"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Wayne"/>
     <s v="sheila@outlook.com"/>
     <s v="The total amount calculation is not accurate, a bit disappointed with this results"/>
-    <x v="2"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Alice"/>
     <s v="sheilalyt@gmail.com"/>
     <s v="Happy to use this application "/>
-    <x v="2"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Bruce"/>
     <s v="sheila@outlook.com"/>
     <s v="Maybe can let us enter more than 3 products in the form in the future for improvement "/>
-    <x v="2"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Sheila"/>
     <s v="sheilalyt@gmail.com"/>
     <s v="Overall staticfied, have space for improvement "/>
-    <x v="2"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Cyan"/>
@@ -1108,74 +347,80 @@
     <s v="t"/>
     <s v="T@"/>
     <s v="hAPPY"/>
-    <x v="3"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="t"/>
     <s v="T"/>
     <s v="Need improvement"/>
-    <x v="3"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="Cyan"/>
     <s v="cyan@gmail.com"/>
     <s v="Disapointed"/>
-    <x v="4"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="Jesmond"/>
     <s v="jesmond@gmail.com"/>
     <s v="Too slow "/>
-    <x v="3"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="Melvin"/>
     <s v="melvin@gmail.com"/>
     <s v="Very happy"/>
-    <x v="5"/>
+    <x v="4"/>
   </r>
   <r>
     <s v="Sheila"/>
     <s v="sheila@gmail.com"/>
     <s v="Disappointed"/>
-    <x v="4"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="Cyan"/>
     <s v="cyan@gmail.com"/>
     <s v="Verrryyyyy happy"/>
-    <x v="3"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="Cyan"/>
     <s v="cyan@gmail.com"/>
     <s v="I am happy to use this service"/>
-    <x v="3"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="Cyan"/>
     <s v="cyan@gmail.com"/>
     <s v="hAPPY"/>
-    <x v="3"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="Cyan"/>
     <s v="cyan@gmail.com"/>
     <s v="hAPPY"/>
-    <x v="3"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="Cyan"/>
     <s v="cyan@gmail.com"/>
-    <s v="Happy_x000a_"/>
-    <x v="6"/>
+    <s v="Need improvement"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Cyan"/>
+    <s v="cyan@gmail.com"/>
+    <s v="Need Improvement but still happy to use this application"/>
+    <x v="0"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0BA0CF26-0DA3-42A1-99AD-00A8C5F86E4C}" name="Pie Data" cacheId="6" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" pageOverThenDown="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1" chartFormat="1">
-  <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CE8951B0-6516-4449-BD1A-4916D9D4BE9C}" name="Pie Data" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" pageOverThenDown="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1" chartFormat="1">
+  <location ref="A1:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0" includeNewItemsInFilter="1">
       <extLst>
@@ -1199,14 +444,12 @@
       </extLst>
     </pivotField>
     <pivotField axis="axisRow" dataField="1" showAll="0" includeNewItemsInFilter="1">
-      <items count="8">
-        <item x="6"/>
-        <item x="4"/>
+      <items count="6">
         <item x="3"/>
+        <item x="2"/>
         <item x="0"/>
         <item x="1"/>
-        <item x="5"/>
-        <item x="2"/>
+        <item x="4"/>
         <item t="default"/>
       </items>
       <extLst>
@@ -1219,7 +462,7 @@
   <rowFields count="1">
     <field x="3"/>
   </rowFields>
-  <rowItems count="8">
+  <rowItems count="6">
     <i>
       <x/>
     </i>
@@ -1234,12 +477,6 @@
     </i>
     <i>
       <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
     </i>
     <i t="grand">
       <x/>
@@ -1571,61 +808,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80E178-60CB-41AE-801C-CD403328AD92}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B8"/>
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
@@ -1633,38 +870,23 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B7" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="4">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,6 +949,9 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1738,6 +963,9 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1749,6 +977,9 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1760,6 +991,9 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1771,6 +1005,9 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1934,10 +1171,24 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
         <v>46</v>
       </c>
-      <c r="D20" t="s">
-        <v>47</v>
+      <c r="D21" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>